<commit_message>
Excel - formating of numbers, CSV - quote encoding
</commit_message>
<xml_diff>
--- a/MethodDemos/output/statistics/cermine-ISSUE.xlsx
+++ b/MethodDemos/output/statistics/cermine-ISSUE.xlsx
@@ -416,75 +416,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
@@ -527,477 +572,483 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
@@ -1019,36 +1070,333 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
@@ -1112,180 +1460,141 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
@@ -1307,1012 +1616,703 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
@@ -2529,8 +2529,8 @@
     <col min="2" max="2" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="2.15234375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="2.15234375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="6.04296875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="8.2734375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="4.35546875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.49609375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="19.921875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.31640625" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="4.9296875" customWidth="true" bestFit="true"/>

</xml_diff>